<commit_message>
Updated University Data 1
</commit_message>
<xml_diff>
--- a/University Data 1.xlsx
+++ b/University Data 1.xlsx
@@ -447,9 +447,6 @@
     <t>1999-09-07</t>
   </si>
   <si>
-    <t>220-04-03</t>
-  </si>
-  <si>
     <t>2006-09-09</t>
   </si>
   <si>
@@ -544,6 +541,9 @@
   </si>
   <si>
     <t>la salle</t>
+  </si>
+  <si>
+    <t>2002-04-03</t>
   </si>
 </sst>
 </file>
@@ -885,8 +885,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -964,7 +964,7 @@
         <v>107</v>
       </c>
       <c r="D5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -978,7 +978,7 @@
         <v>108</v>
       </c>
       <c r="D6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -992,7 +992,7 @@
         <v>109</v>
       </c>
       <c r="D7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1006,7 +1006,7 @@
         <v>110</v>
       </c>
       <c r="D8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1020,7 +1020,7 @@
         <v>111</v>
       </c>
       <c r="D9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1034,7 +1034,7 @@
         <v>112</v>
       </c>
       <c r="D10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1048,7 +1048,7 @@
         <v>113</v>
       </c>
       <c r="D11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1062,7 +1062,7 @@
         <v>114</v>
       </c>
       <c r="D12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1076,7 +1076,7 @@
         <v>115</v>
       </c>
       <c r="D13" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1090,7 +1090,7 @@
         <v>116</v>
       </c>
       <c r="D14" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1104,7 +1104,7 @@
         <v>117</v>
       </c>
       <c r="D15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1118,7 +1118,7 @@
         <v>118</v>
       </c>
       <c r="D16" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1132,7 +1132,7 @@
         <v>119</v>
       </c>
       <c r="D17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1146,7 +1146,7 @@
         <v>120</v>
       </c>
       <c r="D18" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1160,7 +1160,7 @@
         <v>121</v>
       </c>
       <c r="D19" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1188,7 +1188,7 @@
         <v>123</v>
       </c>
       <c r="D21" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1202,7 +1202,7 @@
         <v>124</v>
       </c>
       <c r="D22" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1216,7 +1216,7 @@
         <v>125</v>
       </c>
       <c r="D23" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1230,7 +1230,7 @@
         <v>126</v>
       </c>
       <c r="D24" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1244,7 +1244,7 @@
         <v>127</v>
       </c>
       <c r="D25" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1258,7 +1258,7 @@
         <v>128</v>
       </c>
       <c r="D26" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1272,7 +1272,7 @@
         <v>129</v>
       </c>
       <c r="D27" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1286,7 +1286,7 @@
         <v>130</v>
       </c>
       <c r="D28" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1300,7 +1300,7 @@
         <v>131</v>
       </c>
       <c r="D29" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1314,7 +1314,7 @@
         <v>132</v>
       </c>
       <c r="D30" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1328,7 +1328,7 @@
         <v>133</v>
       </c>
       <c r="D31" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1342,7 +1342,7 @@
         <v>134</v>
       </c>
       <c r="D32" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1356,7 +1356,7 @@
         <v>135</v>
       </c>
       <c r="D33" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1370,7 +1370,7 @@
         <v>136</v>
       </c>
       <c r="D34" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1384,7 +1384,7 @@
         <v>137</v>
       </c>
       <c r="D35" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -1398,7 +1398,7 @@
         <v>138</v>
       </c>
       <c r="D36" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1412,7 +1412,7 @@
         <v>139</v>
       </c>
       <c r="D37" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1426,7 +1426,7 @@
         <v>140</v>
       </c>
       <c r="D38" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1440,7 +1440,7 @@
         <v>141</v>
       </c>
       <c r="D39" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1454,7 +1454,7 @@
         <v>142</v>
       </c>
       <c r="D40" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1465,10 +1465,10 @@
         <v>93</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>143</v>
+        <v>175</v>
       </c>
       <c r="D41" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1479,10 +1479,10 @@
         <v>94</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D42" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1493,10 +1493,10 @@
         <v>95</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D43" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1507,10 +1507,10 @@
         <v>96</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D44" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1521,10 +1521,10 @@
         <v>97</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D45" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1535,10 +1535,10 @@
         <v>98</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D46" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1549,10 +1549,10 @@
         <v>99</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D47" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1563,10 +1563,10 @@
         <v>100</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D48" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1577,10 +1577,10 @@
         <v>101</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D49" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1591,10 +1591,10 @@
         <v>102</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D50" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1605,10 +1605,10 @@
         <v>103</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D51" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>

</xml_diff>